<commit_message>
Create Facebook Test Case
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -1,40 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20385"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pc\Desktop\New folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jomphod.t\Desktop\htmltest\New folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AF3A4AA-A3C8-4240-B09A-10FD811154C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0713ACC2-98C9-4255-9EC1-8F2D09278380}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B497F308-891A-4F29-AA47-67EEF607BB91}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" xr2:uid="{B497F308-891A-4F29-AA47-67EEF607BB91}"/>
   </bookViews>
   <sheets>
-    <sheet name="Login-Logout Module" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="New-Account" sheetId="2" r:id="rId1"/>
+    <sheet name="Login-Logout Module" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="70">
   <si>
     <t>Test Scenario ID</t>
   </si>
@@ -154,22 +146,142 @@
   </si>
   <si>
     <t>TS_FB1</t>
+  </si>
+  <si>
+    <t>TS_FB2</t>
+  </si>
+  <si>
+    <t>TC_FB01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. เปิดเว็บ Facebook
+2. คลิก Create New Account
+</t>
+  </si>
+  <si>
+    <t>แสดงหน้าสมัครสมาชิก</t>
+  </si>
+  <si>
+    <t>TC_FB02</t>
+  </si>
+  <si>
+    <t>TC_FB03</t>
+  </si>
+  <si>
+    <t>TC_FB04</t>
+  </si>
+  <si>
+    <t>TC_FB05</t>
+  </si>
+  <si>
+    <t>TC_FB06</t>
+  </si>
+  <si>
+    <t>TC_FB07</t>
+  </si>
+  <si>
+    <t>สมัครสมาชิก Facebook</t>
+  </si>
+  <si>
+    <t>กรอก First Name และ
+ Surname</t>
+  </si>
+  <si>
+    <t>1. กรอกข้อมูลFirst Name
+2. กรอกข้อมูลSurname</t>
+  </si>
+  <si>
+    <t>กรอก Email Address 
+หรือ Mobile Number</t>
+  </si>
+  <si>
+    <t>1.กรอกข้อมูลEmail</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/</t>
+  </si>
+  <si>
+    <t>First Name: Xxx
+Surname :Xx</t>
+  </si>
+  <si>
+    <t>Email: xxxxx.xx@outlook.com</t>
+  </si>
+  <si>
+    <t>กรอก Password</t>
+  </si>
+  <si>
+    <t>1. กรอก Password</t>
+  </si>
+  <si>
+    <t>Password: xxxxx000000</t>
+  </si>
+  <si>
+    <t>กรอก Date of birth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. เลือกวันที่
+2. เลือกเดือน
+3. เลือกปี คศ
+</t>
+  </si>
+  <si>
+    <t>TC_FB08</t>
+  </si>
+  <si>
+    <t>ยืนยัน Email Address 
+หรือ Mobile Number อีกครั้ง</t>
+  </si>
+  <si>
+    <t>1. กรอกEmail 
+ให้ตรงกับครั้งแรก</t>
+  </si>
+  <si>
+    <t>เลือก Gender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. เลือกเพศ 
+</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>1. กรอกรหัส 5 หลัก
+เพื่อยืนยันบัญชี</t>
+  </si>
+  <si>
+    <t>xxxxx</t>
+  </si>
+  <si>
+    <t>ยืนยันบัญชีFacebook 
+รหัส5หลักถูกส่งไปยัง Email ที่ใช้สมัคร</t>
+  </si>
+  <si>
+    <t>Tc_05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use Logout Facebook </t>
+  </si>
+  <si>
+    <t>1. On click Logout Botton</t>
+  </si>
+  <si>
+    <t>Creat Nem Account Facebook</t>
+  </si>
+  <si>
+    <t>แสดงหน้า Homepage</t>
+  </si>
+  <si>
+    <t>PASS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -198,8 +310,53 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="7"/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -240,50 +397,86 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="15" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -595,174 +788,440 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{855EA4CE-7B83-4B40-AE29-BF0C949402CC}">
-  <dimension ref="A1:I5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B02FD09-3FE7-46EA-957D-696E0B068E0B}">
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="27.85546875" customWidth="1"/>
-    <col min="3" max="3" width="6.5703125" customWidth="1"/>
-    <col min="4" max="4" width="23.7109375" customWidth="1"/>
-    <col min="5" max="5" width="21.140625" customWidth="1"/>
-    <col min="6" max="6" width="29.85546875" customWidth="1"/>
-    <col min="7" max="7" width="52" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.42578125" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="16" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:9" s="3" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="I2" s="5" t="s">
+      <c r="B2" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="I2" s="20" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="1" customFormat="1" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="I3" s="5" t="s">
+    <row r="3" spans="1:9" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="20"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" s="20"/>
+      <c r="H3" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="I3" s="20" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="1" customFormat="1" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="I4" s="5" t="s">
+    <row r="4" spans="1:9" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="20"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="G4" s="20"/>
+      <c r="H4" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="I4" s="20" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="1" customFormat="1" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="I5" s="5" t="s">
+    <row r="5" spans="1:9" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="20"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" s="20"/>
+      <c r="H5" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="I5" s="20" t="s">
         <v>28</v>
       </c>
     </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="20"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="G6" s="20"/>
+      <c r="H6" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="I6" s="20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="20"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" s="22">
+        <v>35202</v>
+      </c>
+      <c r="G7" s="20"/>
+      <c r="H7" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="I7" s="20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="20"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="G8" s="20"/>
+      <c r="H8" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="I8" s="20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="20"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="H9" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="I9" s="20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C10" s="3"/>
+    </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" display="https://en-gb.facebook.com/" xr:uid="{3EE53291-88E2-4BCA-953C-7C4E7DEE9F48}"/>
+    <hyperlink ref="F2" r:id="rId2" xr:uid="{A25B6183-724F-4840-97A4-3DECBF4FADB8}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B02FD09-3FE7-46EA-957D-696E0B068E0B}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{855EA4CE-7B83-4B40-AE29-BF0C949402CC}">
+  <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="27.88671875" customWidth="1"/>
+    <col min="3" max="3" width="6.5546875" customWidth="1"/>
+    <col min="4" max="4" width="23.6640625" customWidth="1"/>
+    <col min="5" max="5" width="21.109375" customWidth="1"/>
+    <col min="6" max="6" width="29.88671875" customWidth="1"/>
+    <col min="7" max="7" width="52" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="1" customFormat="1" ht="51" x14ac:dyDescent="0.3">
+      <c r="A3" s="5"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="1" customFormat="1" ht="51" x14ac:dyDescent="0.3">
+      <c r="A4" s="5"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="1" customFormat="1" ht="51" x14ac:dyDescent="0.3">
+      <c r="A5" s="5"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="4"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="F6" s="14"/>
+      <c r="G6" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>